<commit_message>
add germany combined fertility rates
</commit_message>
<xml_diff>
--- a/notes/to_order.xlsx
+++ b/notes/to_order.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="139">
   <si>
     <t>Country</t>
   </si>
@@ -427,6 +427,12 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/JonMinton/Statistical_Sculpture/master/stl/individual/lmorts/deut_female_(1956-2011).stl</t>
+  </si>
+  <si>
+    <t>https://github.com/JonMinton/Statistical_Sculpture/blob/master/stl/individual/fertility/deut_(1956-2012).stl</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/JonMinton/Statistical_Sculpture/master/stl/individual/fertility/deut_(1956-2012).stl</t>
   </si>
 </sst>
 </file>
@@ -782,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -884,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G57" si="0">D3*E3*F3</f>
+        <f t="shared" ref="G3:G56" si="0">D3*E3*F3</f>
         <v>512</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -1886,10 +1892,10 @@
         <f t="shared" si="0"/>
         <v>512</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="2" t="s">
         <v>136</v>
       </c>
       <c r="J30">
@@ -1923,9 +1929,18 @@
         <f t="shared" si="0"/>
         <v>512</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
       <c r="K31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>512</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2864,11 +2879,11 @@
     <row r="62" spans="1:11">
       <c r="G62">
         <f>SUM(K2:K56)</f>
-        <v>27136</v>
+        <v>27648</v>
       </c>
       <c r="H62">
         <f>G62*0.1</f>
-        <v>2713.6000000000004</v>
+        <v>2764.8</v>
       </c>
       <c r="I62" t="s">
         <v>91</v>
@@ -2877,7 +2892,7 @@
     <row r="63" spans="1:11">
       <c r="H63">
         <f>H62*1.2</f>
-        <v>3256.32</v>
+        <v>3317.76</v>
       </c>
       <c r="I63" t="s">
         <v>92</v>
@@ -2989,9 +3004,13 @@
     <hyperlink ref="I27" r:id="rId102"/>
     <hyperlink ref="I28" r:id="rId103"/>
     <hyperlink ref="I29" r:id="rId104"/>
+    <hyperlink ref="I30" r:id="rId105"/>
+    <hyperlink ref="I31" r:id="rId106"/>
+    <hyperlink ref="H30" r:id="rId107"/>
+    <hyperlink ref="H31" r:id="rId108"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId105"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId109"/>
 </worksheet>
 </file>
 

</xml_diff>